<commit_message>
Remove initial survey screen
</commit_message>
<xml_diff>
--- a/app/config/tables/cold_room_maintenance_logs/forms/cold_room_maintenance_logs/cold_room_maintenance_logs.xlsx
+++ b/app/config/tables/cold_room_maintenance_logs/forms/cold_room_maintenance_logs/cold_room_maintenance_logs.xlsx
@@ -12,13 +12,14 @@
     <workbookView xWindow="11050" yWindow="2690" windowWidth="28370" windowHeight="19560" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" r:id="rId1"/>
-    <sheet name="choices" sheetId="2" r:id="rId2"/>
-    <sheet name="queries" sheetId="3" r:id="rId3"/>
-    <sheet name="settings" sheetId="4" r:id="rId4"/>
-    <sheet name="properties" sheetId="5" r:id="rId5"/>
+    <sheet name="initial" sheetId="6" r:id="rId1"/>
+    <sheet name="survey" sheetId="1" r:id="rId2"/>
+    <sheet name="choices" sheetId="2" r:id="rId3"/>
+    <sheet name="queries" sheetId="3" r:id="rId4"/>
+    <sheet name="settings" sheetId="4" r:id="rId5"/>
+    <sheet name="properties" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="211">
   <si>
     <t>clause</t>
   </si>
@@ -651,6 +652,21 @@
   </si>
   <si>
     <t>birthdate</t>
+  </si>
+  <si>
+    <t>display.text</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>do section survey</t>
+  </si>
+  <si>
+    <t>goto _finalize</t>
+  </si>
+  <si>
+    <t>skips the finalize screen where the user chooses to save as incomplete or finalized and instead saves as finalized</t>
   </si>
 </sst>
 </file>
@@ -1276,9 +1292,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="24.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -1729,7 +1797,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -2073,7 +2141,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -2157,7 +2225,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -2271,7 +2339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>

</xml_diff>

<commit_message>
Change refrigerator, cold room, and maintenance logs to reflect PATH changes
</commit_message>
<xml_diff>
--- a/app/config/tables/cold_room_maintenance_logs/forms/cold_room_maintenance_logs/cold_room_maintenance_logs.xlsx
+++ b/app/config/tables/cold_room_maintenance_logs/forms/cold_room_maintenance_logs/cold_room_maintenance_logs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11050" yWindow="2690" windowWidth="28370" windowHeight="19560" tabRatio="500"/>
+    <workbookView xWindow="11060" yWindow="2690" windowWidth="28370" windowHeight="19560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="6" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="settings" sheetId="4" r:id="rId5"/>
     <sheet name="properties" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="140001"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="272">
   <si>
     <t>clause</t>
   </si>
@@ -76,9 +76,6 @@
     <t>end if</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>date_serviced</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
     <t>Tipo de mantenimiento realizado</t>
   </si>
   <si>
-    <t>select_one</t>
-  </si>
-  <si>
     <t>maint_types</t>
   </si>
   <si>
@@ -301,128 +295,21 @@
     <t>spare_parts</t>
   </si>
   <si>
-    <t>Haga una lista de repuestos</t>
-  </si>
-  <si>
-    <t>Make a list of spare parts</t>
-  </si>
-  <si>
     <t>Select type of maintenance</t>
   </si>
   <si>
     <t>Seleccione el tipo de mantenimiento</t>
   </si>
   <si>
-    <t>addtl_spare_parts</t>
-  </si>
-  <si>
     <t>Spare Parts</t>
   </si>
   <si>
-    <t>Enter additional spare parts</t>
-  </si>
-  <si>
-    <t>Entrar adicional piezas de repuesto</t>
-  </si>
-  <si>
     <t>Piezas de Repuesto</t>
   </si>
   <si>
-    <t>Select spare parts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Seleccione piezas de repuestos</t>
-  </si>
-  <si>
     <t>common_spare_parts</t>
   </si>
   <si>
-    <t>condenser_fan</t>
-  </si>
-  <si>
-    <t>electric_compressor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">charging_cylinder </t>
-  </si>
-  <si>
-    <t>solar_compressor</t>
-  </si>
-  <si>
-    <t>rotary_fan</t>
-  </si>
-  <si>
-    <t>fridge_tag</t>
-  </si>
-  <si>
-    <t>thermostat</t>
-  </si>
-  <si>
-    <t>relay</t>
-  </si>
-  <si>
-    <t>door_gasket</t>
-  </si>
-  <si>
-    <t>Condenser Fan</t>
-  </si>
-  <si>
-    <t>Thermostat</t>
-  </si>
-  <si>
-    <t>Relay</t>
-  </si>
-  <si>
-    <t>Electric Compressor</t>
-  </si>
-  <si>
-    <t>Charging Cylinder</t>
-  </si>
-  <si>
-    <t>Solar Compressor</t>
-  </si>
-  <si>
-    <t>Rotary Fan</t>
-  </si>
-  <si>
-    <t>Fridge Tag</t>
-  </si>
-  <si>
-    <t>Door Gasket</t>
-  </si>
-  <si>
-    <t>Cilindro de carga</t>
-  </si>
-  <si>
-    <t>Ventilador Condensador</t>
-  </si>
-  <si>
-    <t>La Junta de la Puerta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-Compresor Eléctrico</t>
-  </si>
-  <si>
-    <t>Etiqueta Frigorífico</t>
-  </si>
-  <si>
-    <t>Relé</t>
-  </si>
-  <si>
-    <t>Ventilador Rotatorio</t>
-  </si>
-  <si>
-    <t>Compresor Solar</t>
-  </si>
-  <si>
-    <t>Termostato</t>
-  </si>
-  <si>
-    <t>select_multiple_inline</t>
-  </si>
-  <si>
     <t>serviced_by</t>
   </si>
   <si>
@@ -432,21 +319,6 @@
     <t>technician_name</t>
   </si>
   <si>
-    <t>Enter the date of last service</t>
-  </si>
-  <si>
-    <t>Fecha  del último servicio</t>
-  </si>
-  <si>
-    <t>next_date_serviced</t>
-  </si>
-  <si>
-    <t>Next Date Serviced</t>
-  </si>
-  <si>
-    <t>Próxima Fecha de Servicio</t>
-  </si>
-  <si>
     <t>select_multiple</t>
   </si>
   <si>
@@ -513,45 +385,6 @@
     <t>select_one_with_other</t>
   </si>
   <si>
-    <t>fridge_dryer</t>
-  </si>
-  <si>
-    <t>Fridge Dryer</t>
-  </si>
-  <si>
-    <t>electronic_control_unit</t>
-  </si>
-  <si>
-    <t>Electronic Control Unit</t>
-  </si>
-  <si>
-    <t>hinges</t>
-  </si>
-  <si>
-    <t>Hinges</t>
-  </si>
-  <si>
-    <t>need_data</t>
-  </si>
-  <si>
-    <t>Need Data</t>
-  </si>
-  <si>
-    <t>clean_solar_panels</t>
-  </si>
-  <si>
-    <t>Clean solar panels</t>
-  </si>
-  <si>
-    <t>clean_coils</t>
-  </si>
-  <si>
-    <t>Clean coils</t>
-  </si>
-  <si>
-    <t>Necesita Datos</t>
-  </si>
-  <si>
     <t>Garantía / Proveedor de Servicios</t>
   </si>
   <si>
@@ -561,24 +394,6 @@
     <t>Personal de las Facilidades</t>
   </si>
   <si>
-    <t>Secador de Refrigerador</t>
-  </si>
-  <si>
-    <t>Unidad de Control Electrónico</t>
-  </si>
-  <si>
-    <t>Bisagra</t>
-  </si>
-  <si>
-    <t>data('type_of_maintenance') === 'repair'</t>
-  </si>
-  <si>
-    <t>Ingrese la próxima fecha de servicio</t>
-  </si>
-  <si>
-    <t>Enter the next date serviced</t>
-  </si>
-  <si>
     <t>Tipo de Reparación</t>
   </si>
   <si>
@@ -591,9 +406,6 @@
     <t>Seleccione tipo de reparación</t>
   </si>
   <si>
-    <t>Seleccione tipo de mantenimiento</t>
-  </si>
-  <si>
     <t>image</t>
   </si>
   <si>
@@ -606,15 +418,6 @@
     <t>Imagen</t>
   </si>
   <si>
-    <t>Take a picture</t>
-  </si>
-  <si>
-    <t>Toma una foto</t>
-  </si>
-  <si>
-    <t>data('type_of_maintenance') === 'preventative'</t>
-  </si>
-  <si>
     <t>cold_room_maintenance_logs</t>
   </si>
   <si>
@@ -667,19 +470,404 @@
   </si>
   <si>
     <t>skips the finalize screen where the user chooses to save as incomplete or finalized and instead saves as finalized</t>
+  </si>
+  <si>
+    <t>Evaporator Probe</t>
+  </si>
+  <si>
+    <t>Filter Drier</t>
+  </si>
+  <si>
+    <t>High Pressure Switch</t>
+  </si>
+  <si>
+    <t>Low Pressure Switch</t>
+  </si>
+  <si>
+    <t>Compressors</t>
+  </si>
+  <si>
+    <t>evaporator_fan_motor</t>
+  </si>
+  <si>
+    <t>condenser_fan_motor</t>
+  </si>
+  <si>
+    <t>evaporator_probe</t>
+  </si>
+  <si>
+    <t>filter_drier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refrigeration Expansion Valve/Capillary </t>
+  </si>
+  <si>
+    <t>refrigeration_expansive_valve_capillary</t>
+  </si>
+  <si>
+    <t>controllers_complete_with_display</t>
+  </si>
+  <si>
+    <t>high_pressure_switch</t>
+  </si>
+  <si>
+    <t>low_pressure_switch</t>
+  </si>
+  <si>
+    <t>compressors</t>
+  </si>
+  <si>
+    <t>compressor_oil</t>
+  </si>
+  <si>
+    <t>refrigerant_404a</t>
+  </si>
+  <si>
+    <t>Refrigerant 404A - Cylinder gas with 10kg cylinder</t>
+  </si>
+  <si>
+    <t>Motor del ventilador del evaporador</t>
+  </si>
+  <si>
+    <t>Evaporator Fan Motor</t>
+  </si>
+  <si>
+    <t>Condenser Fan Motor</t>
+  </si>
+  <si>
+    <t>Controllers with Display</t>
+  </si>
+  <si>
+    <t>Motor del ventilador del condensador</t>
+  </si>
+  <si>
+    <t>Sonda de evaporador</t>
+  </si>
+  <si>
+    <t>Filtro deshidratador</t>
+  </si>
+  <si>
+    <t>Válvula de expansión de refrigeración/capilar</t>
+  </si>
+  <si>
+    <t>Controladores con pantalla</t>
+  </si>
+  <si>
+    <t>Interruptor de alta presión</t>
+  </si>
+  <si>
+    <t>Interruptor de baja presión</t>
+  </si>
+  <si>
+    <t>Refrigerante 404A - Cilindro de gas con cilindro de 10 kg</t>
+  </si>
+  <si>
+    <t>Compresores</t>
+  </si>
+  <si>
+    <t>Aceite del compresor</t>
+  </si>
+  <si>
+    <t>Compressor Oil</t>
+  </si>
+  <si>
+    <t>technician_phone</t>
+  </si>
+  <si>
+    <t>Technician Phone Number</t>
+  </si>
+  <si>
+    <t>Número de teléfono del técnico</t>
+  </si>
+  <si>
+    <t>Enter technician phone number if available</t>
+  </si>
+  <si>
+    <t>Ingrese el número de teléfono del técnico si está disponible</t>
+  </si>
+  <si>
+    <t>display.title.text.fr</t>
+  </si>
+  <si>
+    <t>display.prompt.text.fr</t>
+  </si>
+  <si>
+    <t>display.locale.text.fr</t>
+  </si>
+  <si>
+    <t>fr</t>
+  </si>
+  <si>
+    <t>Take a picture of the area of repair</t>
+  </si>
+  <si>
+    <t>Tome una fotografía del área de reparación.</t>
+  </si>
+  <si>
+    <t>Enter the date of service</t>
+  </si>
+  <si>
+    <t>Ingrese la fecha de servicio</t>
+  </si>
+  <si>
+    <t>electrical_and_control_system</t>
+  </si>
+  <si>
+    <t>Electrical and Control System</t>
+  </si>
+  <si>
+    <t>Sistema electrico y de control</t>
+  </si>
+  <si>
+    <t>cabinet</t>
+  </si>
+  <si>
+    <t>Cabinet</t>
+  </si>
+  <si>
+    <t>Gabinete</t>
+  </si>
+  <si>
+    <t>refrigeration_system</t>
+  </si>
+  <si>
+    <t>Refrigeration System</t>
+  </si>
+  <si>
+    <t>Sistema de refrigeración</t>
+  </si>
+  <si>
+    <t>power</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power </t>
+  </si>
+  <si>
+    <t>Energía</t>
+  </si>
+  <si>
+    <t>solar</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>temperature_monitoring</t>
+  </si>
+  <si>
+    <t>Temperature Monitoring</t>
+  </si>
+  <si>
+    <t>Monitoreo de temperatura</t>
+  </si>
+  <si>
+    <t>selected(data('type_of_maintenance'), 'other')</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>other_maintenance</t>
+  </si>
+  <si>
+    <t>Other Maintenance</t>
+  </si>
+  <si>
+    <t>Otro mantenimiento</t>
+  </si>
+  <si>
+    <t>Enter other maintenance</t>
+  </si>
+  <si>
+    <t>Ingrese otro mantenimiento</t>
+  </si>
+  <si>
+    <t>selected(data('type_of_repair'), 'other')</t>
+  </si>
+  <si>
+    <t>other_repair</t>
+  </si>
+  <si>
+    <t>Other Repair</t>
+  </si>
+  <si>
+    <t>Otra Reparación</t>
+  </si>
+  <si>
+    <t>Enter other repair</t>
+  </si>
+  <si>
+    <t>Ingrese otra reparación</t>
+  </si>
+  <si>
+    <t>repair_activities</t>
+  </si>
+  <si>
+    <t>Repair Activities</t>
+  </si>
+  <si>
+    <t>Actividades de Reparacion</t>
+  </si>
+  <si>
+    <t>Enter actions taken</t>
+  </si>
+  <si>
+    <t>Ingrese las acciones tomadas</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Enter comments</t>
+  </si>
+  <si>
+    <t>Ingrese comentarios</t>
+  </si>
+  <si>
+    <t>other_spare_parts</t>
+  </si>
+  <si>
+    <t>Other spare parts replaced/used</t>
+  </si>
+  <si>
+    <t>Otras piezas de repuesto reemplazadas/usadas</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Actualizar estado del refrigerador</t>
+  </si>
+  <si>
+    <t>French</t>
+  </si>
+  <si>
+    <t>Francés</t>
+  </si>
+  <si>
+    <t>Francais</t>
+  </si>
+  <si>
+    <t>Anglais</t>
+  </si>
+  <si>
+    <t>Espagnol</t>
+  </si>
+  <si>
+    <t>Update Cold Room Status</t>
+  </si>
+  <si>
+    <t>Please update cold room status as needed</t>
+  </si>
+  <si>
+    <t>Actualice el estado del cuarto frio según sea necesario</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
+  </si>
+  <si>
+    <t>preventative_comments</t>
+  </si>
+  <si>
+    <t>Select spare parts replaced/used</t>
+  </si>
+  <si>
+    <t>Seleccione piezas de repuestos reemplazadas/usadas</t>
+  </si>
+  <si>
+    <t>selected(data('type_of_maintenance'), 'repair')</t>
+  </si>
+  <si>
+    <t>selected(data('type_of_maintenance'), 'preventative')</t>
+  </si>
+  <si>
+    <t>Select type of preventative maintenance</t>
+  </si>
+  <si>
+    <t>Seleccione tipo de mantenimiento preventivo</t>
+  </si>
+  <si>
+    <t>Check evaporator</t>
+  </si>
+  <si>
+    <t>Check duty-sharing system</t>
+  </si>
+  <si>
+    <t>Check enclosure</t>
+  </si>
+  <si>
+    <t>Check door and lock</t>
+  </si>
+  <si>
+    <t>Check freezer pressure release vent</t>
+  </si>
+  <si>
+    <t>Check spare parts inventory</t>
+  </si>
+  <si>
+    <t>check_evaporator</t>
+  </si>
+  <si>
+    <t>check_duty_sharing_system</t>
+  </si>
+  <si>
+    <t>Check temperature monitoring system</t>
+  </si>
+  <si>
+    <t>check_temperature_monitoring_system</t>
+  </si>
+  <si>
+    <t>check_enclosure</t>
+  </si>
+  <si>
+    <t>check_door_and_lock</t>
+  </si>
+  <si>
+    <t>check_freezer_pressure_release_vent</t>
+  </si>
+  <si>
+    <t>check_spare_parts_inventory</t>
+  </si>
+  <si>
+    <t>Comprobar evaporador</t>
+  </si>
+  <si>
+    <t>Comprobar el sistema de reparto de tareas</t>
+  </si>
+  <si>
+    <t>Comprobar el sistema de monitoreo de temperatura</t>
+  </si>
+  <si>
+    <t>Comprobar el recinto</t>
+  </si>
+  <si>
+    <t>Comprobar puerta y cerradura</t>
+  </si>
+  <si>
+    <t>Comprobar ventilación de liberación de presión del congelador</t>
+  </si>
+  <si>
+    <t>Comprobar inventario de repuestos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -714,17 +902,20 @@
     <font>
       <sz val="11"/>
       <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF212121"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -770,54 +961,55 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="40">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -827,7 +1019,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -835,19 +1027,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="40">
+  <cellStyles count="41">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -888,6 +1087,7 @@
     <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="40"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1294,7 +1494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1313,27 +1513,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>206</v>
+        <v>141</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>207</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>208</v>
+        <v>143</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>209</v>
+        <v>144</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>210</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1344,27 +1544,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.9140625" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="22.58203125" customWidth="1"/>
     <col min="5" max="5" width="20.58203125" customWidth="1"/>
-    <col min="6" max="6" width="32.9140625" customWidth="1"/>
-    <col min="7" max="7" width="32.4140625" customWidth="1"/>
-    <col min="8" max="8" width="24.58203125" customWidth="1"/>
-    <col min="9" max="9" width="39.5" customWidth="1"/>
-    <col min="10" max="1025" width="8.5" customWidth="1"/>
+    <col min="6" max="6" width="32.83203125" customWidth="1"/>
+    <col min="7" max="8" width="32.33203125" customWidth="1"/>
+    <col min="9" max="9" width="24.58203125" customWidth="1"/>
+    <col min="10" max="11" width="39.5" customWidth="1"/>
+    <col min="12" max="1027" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1387,16 +1587,22 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1408,8 +1614,10 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1423,8 +1631,10 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -1432,25 +1642,25 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s">
-        <v>200</v>
+        <v>135</v>
       </c>
       <c r="F4" t="s">
-        <v>201</v>
+        <v>136</v>
       </c>
       <c r="G4" t="s">
-        <v>202</v>
-      </c>
-      <c r="H4" t="s">
-        <v>203</v>
+        <v>137</v>
       </c>
       <c r="I4" t="s">
-        <v>204</v>
-      </c>
-      <c r="J4">
+        <v>138</v>
+      </c>
+      <c r="J4" t="s">
+        <v>139</v>
+      </c>
+      <c r="L4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1461,33 +1671,37 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>130</v>
+        <v>93</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>129</v>
+        <v>92</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>144</v>
+        <v>102</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="K6" s="14"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
@@ -1495,295 +1709,456 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="1" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>148</v>
+        <v>106</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>151</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>181</v>
+      </c>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="31" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>186</v>
-      </c>
+      <c r="C9" s="1"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" ht="31" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="17" t="s">
         <v>188</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C11" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="I11" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C12" s="3" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3" t="s">
-        <v>134</v>
+        <v>14</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>135</v>
+        <v>15</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="J12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>12</v>
       </c>
       <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
         <v>18</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>19</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>20</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
         <v>21</v>
       </c>
-      <c r="I13" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" t="s">
         <v>74</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>75</v>
       </c>
-      <c r="G14" t="s">
-        <v>76</v>
-      </c>
-      <c r="H14" t="s">
-        <v>91</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I14" t="s">
+        <v>87</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="C15" s="1"/>
-      <c r="I15" s="9"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C16" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D16" t="s">
-        <v>138</v>
+        <v>210</v>
       </c>
       <c r="E16" t="s">
-        <v>139</v>
+        <v>211</v>
       </c>
       <c r="F16" t="s">
-        <v>140</v>
+        <v>212</v>
       </c>
       <c r="G16" t="s">
-        <v>181</v>
-      </c>
-      <c r="H16" t="s">
-        <v>183</v>
-      </c>
-      <c r="I16" s="9" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>213</v>
+      </c>
+      <c r="I16" t="s">
+        <v>214</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="I17" s="9"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>192</v>
+        <v>247</v>
       </c>
       <c r="C18" s="1"/>
-      <c r="I18" s="9"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C19" s="1" t="s">
-        <v>137</v>
+        <v>95</v>
       </c>
       <c r="D19" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
       <c r="E19" t="s">
-        <v>142</v>
+        <v>97</v>
       </c>
       <c r="F19" t="s">
-        <v>143</v>
+        <v>98</v>
       </c>
       <c r="G19" t="s">
-        <v>182</v>
-      </c>
-      <c r="H19" t="s">
+        <v>120</v>
+      </c>
+      <c r="I19" t="s">
+        <v>122</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="K19" s="9"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>216</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C21" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E21" t="s">
+        <v>217</v>
+      </c>
+      <c r="F21" t="s">
+        <v>218</v>
+      </c>
+      <c r="G21" t="s">
+        <v>219</v>
+      </c>
+      <c r="I21" t="s">
+        <v>220</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="K21" s="9"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C23" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E23" t="s">
+        <v>222</v>
+      </c>
+      <c r="F23" t="s">
+        <v>223</v>
+      </c>
+      <c r="G23" t="s">
+        <v>224</v>
+      </c>
+      <c r="I23" t="s">
+        <v>225</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="K23" s="9"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>248</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C26" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D26" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" t="s">
+        <v>100</v>
+      </c>
+      <c r="F26" t="s">
+        <v>101</v>
+      </c>
+      <c r="G26" t="s">
+        <v>121</v>
+      </c>
+      <c r="I26" t="s">
+        <v>249</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="K26" s="9"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C27" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27" t="s">
+        <v>244</v>
+      </c>
+      <c r="F27" t="s">
+        <v>227</v>
+      </c>
+      <c r="G27" t="s">
+        <v>243</v>
+      </c>
+      <c r="I27" t="s">
+        <v>228</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="K27" s="9"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+    </row>
+    <row r="31" spans="1:11" ht="31" x14ac:dyDescent="0.35">
+      <c r="C31" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" t="s">
         <v>91</v>
       </c>
-      <c r="I19" s="9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="I20" s="9"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="I21" s="9"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="1"/>
-      <c r="I22" s="9"/>
-    </row>
-    <row r="23" spans="1:9" ht="31" x14ac:dyDescent="0.35">
-      <c r="C23" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D23" t="s">
-        <v>100</v>
-      </c>
-      <c r="E23" t="s">
-        <v>88</v>
-      </c>
-      <c r="F23" t="s">
-        <v>94</v>
-      </c>
-      <c r="G23" t="s">
-        <v>97</v>
-      </c>
-      <c r="H23" t="s">
-        <v>98</v>
-      </c>
-      <c r="I23" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="C24" s="1" t="s">
+      <c r="E31" t="s">
+        <v>86</v>
+      </c>
+      <c r="F31" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" t="s">
+        <v>90</v>
+      </c>
+      <c r="I31" t="s">
+        <v>245</v>
+      </c>
+      <c r="J31" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="K31" s="9"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C32" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E24" t="s">
-        <v>93</v>
-      </c>
-      <c r="F24" t="s">
-        <v>95</v>
-      </c>
-      <c r="G24" t="s">
-        <v>96</v>
-      </c>
-      <c r="H24" t="s">
-        <v>90</v>
-      </c>
-      <c r="I24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>23</v>
+      <c r="E32" t="s">
+        <v>230</v>
+      </c>
+      <c r="F32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G32" t="s">
+        <v>85</v>
+      </c>
+      <c r="I32" t="s">
+        <v>231</v>
+      </c>
+      <c r="J32" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C34" t="s">
+        <v>233</v>
+      </c>
+      <c r="F34" t="s">
+        <v>240</v>
+      </c>
+      <c r="G34" t="s">
+        <v>234</v>
+      </c>
+      <c r="I34" t="s">
+        <v>241</v>
+      </c>
+      <c r="J34" t="s">
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -1799,27 +2174,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23.08203125" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="18.4140625" customWidth="1"/>
-    <col min="4" max="4" width="20.4140625" customWidth="1"/>
+    <col min="2" max="2" width="32.83203125" customWidth="1"/>
+    <col min="3" max="3" width="39.25" customWidth="1"/>
+    <col min="4" max="4" width="45.5" customWidth="1"/>
     <col min="5" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -1827,308 +2202,461 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
         <v>78</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
         <v>82</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" t="s">
         <v>79</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>130</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" t="s">
+        <v>165</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C11" t="s">
+        <v>166</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" t="s">
+        <v>147</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C15" t="s">
+        <v>167</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B7" t="s">
-        <v>154</v>
-      </c>
-      <c r="C7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="C16" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>130</v>
-      </c>
-      <c r="B8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D8" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>100</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="C11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>100</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>100</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C14" t="s">
-        <v>117</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="C15" t="s">
-        <v>112</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>100</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>107</v>
+        <v>162</v>
       </c>
       <c r="C18" t="s">
-        <v>111</v>
+        <v>163</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>159</v>
+        <v>91</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>160</v>
       </c>
       <c r="C19" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>100</v>
-      </c>
-      <c r="B20" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>161</v>
       </c>
       <c r="C20" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="C21" t="s">
-        <v>164</v>
-      </c>
-      <c r="D21" s="16" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="C22" t="s">
+        <v>193</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E22" s="18"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>138</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>165</v>
+        <v>96</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>195</v>
       </c>
       <c r="C23" t="s">
-        <v>166</v>
+        <v>196</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+        <v>197</v>
+      </c>
+      <c r="E23" s="18"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>96</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="C24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>141</v>
-      </c>
-      <c r="B25" t="s">
-        <v>167</v>
+        <v>96</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>201</v>
       </c>
       <c r="C25" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+        <v>202</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>141</v>
-      </c>
-      <c r="B26" t="s">
-        <v>169</v>
+        <v>96</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>204</v>
       </c>
       <c r="C26" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+        <v>205</v>
+      </c>
+      <c r="D26" t="s">
+        <v>205</v>
+      </c>
+      <c r="E26" s="18"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>141</v>
-      </c>
-      <c r="B27" t="s">
-        <v>165</v>
+        <v>96</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>206</v>
       </c>
       <c r="C27" t="s">
-        <v>166</v>
+        <v>207</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>171</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="E27" s="18"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C28" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="18"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B29" s="15"/>
+      <c r="D29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="D30" t="s">
+        <v>265</v>
+      </c>
+      <c r="E30" s="18"/>
+    </row>
+    <row r="31" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="E31" s="18"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="E32" s="18"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="E33" s="18"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="E34" s="18"/>
+    </row>
+    <row r="35" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="E35" s="18"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>256</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="E36" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2149,69 +2677,69 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="23.4140625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
-    <col min="5" max="5" width="29.9140625" customWidth="1"/>
+    <col min="5" max="5" width="29.83203125" customWidth="1"/>
     <col min="6" max="6" width="35" customWidth="1"/>
     <col min="7" max="7" width="47.08203125" customWidth="1"/>
-    <col min="8" max="8" width="38.9140625" customWidth="1"/>
+    <col min="8" max="8" width="38.83203125" customWidth="1"/>
     <col min="9" max="1025" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" t="s">
-        <v>199</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -2227,28 +2755,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="8.5" customWidth="1"/>
-    <col min="3" max="3" width="19.9140625" customWidth="1"/>
-    <col min="4" max="4" width="17.08203125" customWidth="1"/>
-    <col min="5" max="5" width="29.08203125" customWidth="1"/>
-    <col min="6" max="1025" width="8.5" customWidth="1"/>
+    <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="5" width="17.08203125" customWidth="1"/>
+    <col min="6" max="6" width="18.25" customWidth="1"/>
+    <col min="7" max="7" width="18.08203125" customWidth="1"/>
+    <col min="8" max="8" width="19.08203125" customWidth="1"/>
+    <col min="9" max="1026" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>38</v>
-      </c>
-      <c r="B1" t="s">
-        <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -2257,75 +2787,101 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
         <v>40</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="C4" t="s">
-        <v>194</v>
-      </c>
-      <c r="D4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="B5" s="6">
         <v>20191005</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="F7" t="s">
         <v>47</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>48</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" s="18" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="F8" t="s">
         <v>50</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>51</v>
       </c>
-      <c r="F8" t="s">
-        <v>52</v>
+      <c r="H8" s="18" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>187</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>235</v>
+      </c>
+      <c r="G9" t="s">
+        <v>236</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2347,7 +2903,7 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="8.5" customWidth="1"/>
     <col min="3" max="3" width="22.58203125" customWidth="1"/>
@@ -2358,138 +2914,138 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>57</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>58</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="C3" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>196</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="C4" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>197</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove all pictures except refrigerator serial number and indicators survey pictures
</commit_message>
<xml_diff>
--- a/app/config/tables/cold_room_maintenance_logs/forms/cold_room_maintenance_logs/cold_room_maintenance_logs.xlsx
+++ b/app/config/tables/cold_room_maintenance_logs/forms/cold_room_maintenance_logs/cold_room_maintenance_logs.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="266">
   <si>
     <t>clause</t>
   </si>
@@ -406,18 +406,6 @@
     <t>Seleccione tipo de reparación</t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>maintenance_log_image</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>Imagen</t>
-  </si>
-  <si>
     <t>cold_room_maintenance_logs</t>
   </si>
   <si>
@@ -596,12 +584,6 @@
   </si>
   <si>
     <t>fr</t>
-  </si>
-  <si>
-    <t>Take a picture of the area of repair</t>
-  </si>
-  <si>
-    <t>Tome una fotografía del área de reparación.</t>
   </si>
   <si>
     <t>Enter the date of service</t>
@@ -1004,7 +986,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1038,9 +1020,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1513,27 +1492,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1544,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1587,7 +1566,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -1596,7 +1575,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -1642,19 +1621,19 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" t="s">
+        <v>133</v>
+      </c>
+      <c r="I4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" t="s">
         <v>135</v>
-      </c>
-      <c r="F4" t="s">
-        <v>136</v>
-      </c>
-      <c r="G4" t="s">
-        <v>137</v>
-      </c>
-      <c r="I4" t="s">
-        <v>138</v>
-      </c>
-      <c r="J4" t="s">
-        <v>139</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -1734,20 +1713,20 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="J8" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -1765,315 +1744,298 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:12" ht="31" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>124</v>
-      </c>
+      <c r="C10" s="1"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>127</v>
-      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>189</v>
-      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="C11" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="J11" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C12" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3" t="s">
-        <v>190</v>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" t="s">
+        <v>20</v>
       </c>
       <c r="J12" t="s">
-        <v>191</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C13" t="s">
-        <v>12</v>
+      <c r="C13" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" t="s">
+        <v>76</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="G13" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="I13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" t="s">
-        <v>21</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C14" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D14" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" t="s">
-        <v>75</v>
-      </c>
-      <c r="I14" t="s">
-        <v>87</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>88</v>
-      </c>
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>203</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="J14" s="9"/>
       <c r="K14" s="9"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C15" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E15" t="s">
+        <v>205</v>
+      </c>
+      <c r="F15" t="s">
+        <v>206</v>
+      </c>
+      <c r="G15" t="s">
+        <v>207</v>
+      </c>
+      <c r="I15" t="s">
+        <v>208</v>
+      </c>
+      <c r="J15" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="J15" s="9"/>
       <c r="K15" s="9"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C16" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E16" t="s">
-        <v>211</v>
-      </c>
-      <c r="F16" t="s">
-        <v>212</v>
-      </c>
-      <c r="G16" t="s">
-        <v>213</v>
-      </c>
-      <c r="I16" t="s">
-        <v>214</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>215</v>
-      </c>
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="J16" s="9"/>
       <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>241</v>
       </c>
       <c r="C17" s="1"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="C18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" t="s">
+        <v>120</v>
+      </c>
+      <c r="I18" t="s">
+        <v>122</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="K18" s="9"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="B18" t="s">
-        <v>247</v>
-      </c>
-      <c r="C18" s="1"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C19" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E19" t="s">
-        <v>97</v>
-      </c>
-      <c r="F19" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" t="s">
-        <v>120</v>
-      </c>
-      <c r="I19" t="s">
-        <v>122</v>
-      </c>
-      <c r="J19" s="9" t="s">
-        <v>123</v>
-      </c>
+      <c r="B19" t="s">
+        <v>210</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="J19" s="9"/>
       <c r="K19" s="9"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C20" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E20" t="s">
+        <v>211</v>
+      </c>
+      <c r="F20" t="s">
+        <v>212</v>
+      </c>
+      <c r="G20" t="s">
+        <v>213</v>
+      </c>
+      <c r="I20" t="s">
+        <v>214</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="K20" s="9"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C22" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="E22" t="s">
         <v>216</v>
       </c>
-      <c r="C20" s="1"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C21" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F22" t="s">
         <v>217</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G22" t="s">
         <v>218</v>
       </c>
-      <c r="G21" t="s">
+      <c r="I22" t="s">
         <v>219</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J22" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="J21" s="9" t="s">
-        <v>221</v>
-      </c>
-      <c r="K21" s="9"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="K22" s="9"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="1"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C23" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E23" t="s">
-        <v>222</v>
-      </c>
-      <c r="F23" t="s">
-        <v>223</v>
-      </c>
-      <c r="G23" t="s">
-        <v>224</v>
-      </c>
-      <c r="I23" t="s">
-        <v>225</v>
-      </c>
-      <c r="J23" s="9" t="s">
-        <v>226</v>
-      </c>
+      <c r="C23" s="1"/>
+      <c r="J23" s="9"/>
       <c r="K23" s="9"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>242</v>
       </c>
       <c r="C24" s="1"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" t="s">
-        <v>248</v>
-      </c>
-      <c r="C25" s="1"/>
-      <c r="J25" s="9"/>
+      <c r="C25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D25" t="s">
+        <v>99</v>
+      </c>
+      <c r="E25" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" t="s">
+        <v>121</v>
+      </c>
+      <c r="I25" t="s">
+        <v>243</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>244</v>
+      </c>
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C26" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D26" t="s">
-        <v>99</v>
+        <v>204</v>
       </c>
       <c r="E26" t="s">
-        <v>100</v>
+        <v>238</v>
       </c>
       <c r="F26" t="s">
-        <v>101</v>
+        <v>221</v>
       </c>
       <c r="G26" t="s">
-        <v>121</v>
+        <v>237</v>
       </c>
       <c r="I26" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="K26" s="9"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C27" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E27" t="s">
-        <v>244</v>
-      </c>
-      <c r="F27" t="s">
-        <v>227</v>
-      </c>
-      <c r="G27" t="s">
-        <v>243</v>
-      </c>
-      <c r="I27" t="s">
-        <v>228</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>229</v>
-      </c>
+      <c r="A27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="J27" s="9"/>
       <c r="K27" s="9"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C28" s="1"/>
       <c r="J28" s="9"/>
@@ -2081,84 +2043,76 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C29" s="1"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="1"/>
-      <c r="J30" s="9"/>
+    <row r="30" spans="1:11" ht="31" x14ac:dyDescent="0.35">
+      <c r="C30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D30" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" t="s">
+        <v>86</v>
+      </c>
+      <c r="F30" t="s">
+        <v>89</v>
+      </c>
+      <c r="G30" t="s">
+        <v>90</v>
+      </c>
+      <c r="I30" t="s">
+        <v>239</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>240</v>
+      </c>
       <c r="K30" s="9"/>
     </row>
-    <row r="31" spans="1:11" ht="31" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C31" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D31" t="s">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>86</v>
+        <v>224</v>
       </c>
       <c r="F31" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="G31" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I31" t="s">
-        <v>245</v>
-      </c>
-      <c r="J31" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="K31" s="9"/>
+        <v>225</v>
+      </c>
+      <c r="J31" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" t="s">
-        <v>230</v>
-      </c>
-      <c r="F32" t="s">
-        <v>79</v>
-      </c>
-      <c r="G32" t="s">
-        <v>85</v>
-      </c>
-      <c r="I32" t="s">
-        <v>231</v>
-      </c>
-      <c r="J32" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+      <c r="A32" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="C34" t="s">
-        <v>233</v>
-      </c>
-      <c r="F34" t="s">
-        <v>240</v>
-      </c>
-      <c r="G34" t="s">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.35">
+      <c r="C33" t="s">
+        <v>227</v>
+      </c>
+      <c r="F33" t="s">
         <v>234</v>
       </c>
-      <c r="I34" t="s">
-        <v>241</v>
-      </c>
-      <c r="J34" t="s">
-        <v>242</v>
+      <c r="G33" t="s">
+        <v>228</v>
+      </c>
+      <c r="I33" t="s">
+        <v>235</v>
+      </c>
+      <c r="J33" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2203,7 +2157,7 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -2295,13 +2249,13 @@
         <v>91</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -2309,13 +2263,13 @@
         <v>91</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -2323,13 +2277,13 @@
         <v>91</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C12" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -2337,13 +2291,13 @@
         <v>91</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -2351,13 +2305,13 @@
         <v>91</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C14" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -2365,13 +2319,13 @@
         <v>91</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C15" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
@@ -2379,13 +2333,13 @@
         <v>91</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C16" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
@@ -2393,13 +2347,13 @@
         <v>91</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -2407,13 +2361,13 @@
         <v>91</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C18" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -2421,13 +2375,13 @@
         <v>91</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
@@ -2435,13 +2389,13 @@
         <v>91</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C20" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D20" s="16" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
@@ -2449,90 +2403,90 @@
         <v>96</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C22" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="E22" s="18"/>
+        <v>188</v>
+      </c>
+      <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>96</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C23" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="E23" s="18"/>
+        <v>191</v>
+      </c>
+      <c r="E23" s="17"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>96</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="C24" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="E24" s="18"/>
+        <v>194</v>
+      </c>
+      <c r="E24" s="17"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>96</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="C25" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>203</v>
-      </c>
-      <c r="E25" s="18"/>
+        <v>197</v>
+      </c>
+      <c r="E25" s="17"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>96</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C26" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D26" t="s">
-        <v>205</v>
-      </c>
-      <c r="E26" s="18"/>
+        <v>199</v>
+      </c>
+      <c r="E26" s="17"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>96</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C27" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="E27" s="18"/>
+        <v>202</v>
+      </c>
+      <c r="E27" s="17"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
@@ -2547,7 +2501,7 @@
       <c r="D28" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E28" s="18"/>
+      <c r="E28" s="17"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B29" s="15"/>
@@ -2558,105 +2512,105 @@
         <v>99</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C30" s="19" t="s">
         <v>251</v>
       </c>
+      <c r="C30" s="18" t="s">
+        <v>245</v>
+      </c>
       <c r="D30" t="s">
-        <v>265</v>
-      </c>
-      <c r="E30" s="18"/>
+        <v>259</v>
+      </c>
+      <c r="E30" s="17"/>
     </row>
     <row r="31" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>99</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="C31" s="19" t="s">
         <v>252</v>
       </c>
+      <c r="C31" s="18" t="s">
+        <v>246</v>
+      </c>
       <c r="D31" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="E31" s="18"/>
+        <v>260</v>
+      </c>
+      <c r="E31" s="17"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>99</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>260</v>
-      </c>
-      <c r="C32" s="19" t="s">
-        <v>259</v>
+        <v>254</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>253</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="E32" s="18"/>
+        <v>261</v>
+      </c>
+      <c r="E32" s="17"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>99</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="C33" s="19" t="s">
-        <v>253</v>
+        <v>255</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>247</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>268</v>
-      </c>
-      <c r="E33" s="18"/>
+        <v>262</v>
+      </c>
+      <c r="E33" s="17"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>99</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>262</v>
-      </c>
-      <c r="C34" s="19" t="s">
-        <v>254</v>
+        <v>256</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>248</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="E34" s="18"/>
+        <v>263</v>
+      </c>
+      <c r="E34" s="17"/>
     </row>
     <row r="35" spans="1:5" ht="31" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>99</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>255</v>
+        <v>257</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>249</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="E35" s="18"/>
+        <v>264</v>
+      </c>
+      <c r="E35" s="17"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>99</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>256</v>
+        <v>258</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>250</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="E36" s="18"/>
+        <v>265</v>
+      </c>
+      <c r="E36" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2718,16 +2672,16 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E2" t="s">
         <v>34</v>
@@ -2787,7 +2741,7 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F1" t="s">
         <v>39</v>
@@ -2796,7 +2750,7 @@
         <v>40</v>
       </c>
       <c r="H1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -2804,7 +2758,7 @@
         <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -2812,7 +2766,7 @@
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -2820,10 +2774,10 @@
         <v>43</v>
       </c>
       <c r="C4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -2852,8 +2806,8 @@
       <c r="G7" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="18" t="s">
-        <v>238</v>
+      <c r="H7" s="17" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -2866,22 +2820,22 @@
       <c r="G8" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="18" t="s">
-        <v>239</v>
+      <c r="H8" s="17" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>235</v>
+        <v>183</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>229</v>
       </c>
       <c r="G9" t="s">
-        <v>236</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>237</v>
+        <v>230</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -2960,7 +2914,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -2977,7 +2931,7 @@
         <v>12</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Change preventative maintenance choice options text
</commit_message>
<xml_diff>
--- a/app/config/tables/cold_room_maintenance_logs/forms/cold_room_maintenance_logs/cold_room_maintenance_logs.xlsx
+++ b/app/config/tables/cold_room_maintenance_logs/forms/cold_room_maintenance_logs/cold_room_maintenance_logs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="2690" windowWidth="28370" windowHeight="19560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="11060" yWindow="2690" windowWidth="28370" windowHeight="19560" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="6" r:id="rId1"/>
@@ -769,33 +769,12 @@
     <t>Seleccione tipo de mantenimiento preventivo</t>
   </si>
   <si>
-    <t>Check evaporator</t>
-  </si>
-  <si>
-    <t>Check duty-sharing system</t>
-  </si>
-  <si>
-    <t>Check enclosure</t>
-  </si>
-  <si>
-    <t>Check door and lock</t>
-  </si>
-  <si>
-    <t>Check freezer pressure release vent</t>
-  </si>
-  <si>
-    <t>Check spare parts inventory</t>
-  </si>
-  <si>
     <t>check_evaporator</t>
   </si>
   <si>
     <t>check_duty_sharing_system</t>
   </si>
   <si>
-    <t>Check temperature monitoring system</t>
-  </si>
-  <si>
     <t>check_temperature_monitoring_system</t>
   </si>
   <si>
@@ -811,25 +790,46 @@
     <t>check_spare_parts_inventory</t>
   </si>
   <si>
-    <t>Comprobar evaporador</t>
-  </si>
-  <si>
-    <t>Comprobar el sistema de reparto de tareas</t>
-  </si>
-  <si>
-    <t>Comprobar el sistema de monitoreo de temperatura</t>
-  </si>
-  <si>
-    <t>Comprobar el recinto</t>
-  </si>
-  <si>
-    <t>Comprobar puerta y cerradura</t>
-  </si>
-  <si>
-    <t>Comprobar ventilación de liberación de presión del congelador</t>
-  </si>
-  <si>
-    <t>Comprobar inventario de repuestos</t>
+    <t>Check/clean/tighten evaporator</t>
+  </si>
+  <si>
+    <t>Check/clean/tighten duty-sharing system</t>
+  </si>
+  <si>
+    <t>Check/clean/tighten temperature monitoring system</t>
+  </si>
+  <si>
+    <t>Check/clean/tighten enclosure</t>
+  </si>
+  <si>
+    <t>Check/clean/tighten door and lock</t>
+  </si>
+  <si>
+    <t>Check/clean/tighten freezer pressure release vent</t>
+  </si>
+  <si>
+    <t>Check/clean/tighten spare parts inventory</t>
+  </si>
+  <si>
+    <t>Comprobar/limpiar/apretar evaporador</t>
+  </si>
+  <si>
+    <t>Comprobar/limpiar/apretar el sistema de reparto de tareas</t>
+  </si>
+  <si>
+    <t>Comprobar/limpiar/apretar el sistema de monitoreo de temperatura</t>
+  </si>
+  <si>
+    <t>Comprobar/limpiar/apretar el recinto</t>
+  </si>
+  <si>
+    <t>Comprobar/limpiar/apretar puerta y cerradura</t>
+  </si>
+  <si>
+    <t>Comprobar/limpiar/apretar ventilación de liberación de presión del congelador</t>
+  </si>
+  <si>
+    <t>Comprobar/limpiar/apretar inventario de repuestos</t>
   </si>
 </sst>
 </file>
@@ -920,7 +920,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -931,6 +931,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFABF8F"/>
         <bgColor rgb="FFFF99CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -986,7 +992,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1021,8 +1027,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="41">
@@ -1525,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2130,13 +2141,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.08203125" customWidth="1"/>
+    <col min="1" max="1" width="29.83203125" customWidth="1"/>
     <col min="2" max="2" width="32.83203125" customWidth="1"/>
     <col min="3" max="3" width="39.25" customWidth="1"/>
     <col min="4" max="4" width="45.5" customWidth="1"/>
@@ -2507,110 +2518,103 @@
       <c r="B29" s="15"/>
       <c r="D29" s="9"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="30" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="C30" s="20" t="s">
+        <v>252</v>
+      </c>
+      <c r="D30" s="18" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="18" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>246</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="18" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A32" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="C32" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="D32" s="21" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="D33" s="21" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>249</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>256</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="18" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="A35" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="C35" s="20" t="s">
+        <v>257</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="D30" t="s">
-        <v>259</v>
-      </c>
-      <c r="E30" s="17"/>
-    </row>
-    <row r="31" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="E31" s="17"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>99</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>253</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>261</v>
-      </c>
-      <c r="E32" s="17"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>99</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="E33" s="17"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>248</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="E34" s="17"/>
-    </row>
-    <row r="35" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>99</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>249</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="E35" s="17"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" s="10" t="s">
+      <c r="C36" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="C36" s="18" t="s">
-        <v>250</v>
-      </c>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="21" t="s">
         <v>265</v>
       </c>
-      <c r="E36" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Change spare parts list for cold room maintenace logs
</commit_message>
<xml_diff>
--- a/app/config/tables/cold_room_maintenance_logs/forms/cold_room_maintenance_logs/cold_room_maintenance_logs.xlsx
+++ b/app/config/tables/cold_room_maintenance_logs/forms/cold_room_maintenance_logs/cold_room_maintenance_logs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="2690" windowWidth="28370" windowHeight="19560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="11060" yWindow="2690" windowWidth="28370" windowHeight="19560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="263">
   <si>
     <t>clause</t>
   </si>
@@ -466,12 +466,6 @@
     <t>Filter Drier</t>
   </si>
   <si>
-    <t>High Pressure Switch</t>
-  </si>
-  <si>
-    <t>Low Pressure Switch</t>
-  </si>
-  <si>
     <t>Compressors</t>
   </si>
   <si>
@@ -496,24 +490,12 @@
     <t>controllers_complete_with_display</t>
   </si>
   <si>
-    <t>high_pressure_switch</t>
-  </si>
-  <si>
-    <t>low_pressure_switch</t>
-  </si>
-  <si>
     <t>compressors</t>
   </si>
   <si>
     <t>compressor_oil</t>
   </si>
   <si>
-    <t>refrigerant_404a</t>
-  </si>
-  <si>
-    <t>Refrigerant 404A - Cylinder gas with 10kg cylinder</t>
-  </si>
-  <si>
     <t>Motor del ventilador del evaporador</t>
   </si>
   <si>
@@ -541,15 +523,6 @@
     <t>Controladores con pantalla</t>
   </si>
   <si>
-    <t>Interruptor de alta presión</t>
-  </si>
-  <si>
-    <t>Interruptor de baja presión</t>
-  </si>
-  <si>
-    <t>Refrigerante 404A - Cilindro de gas con cilindro de 10 kg</t>
-  </si>
-  <si>
     <t>Compresores</t>
   </si>
   <si>
@@ -830,6 +803,24 @@
   </si>
   <si>
     <t>Comprobar/limpiar/apretar inventario de repuestos</t>
+  </si>
+  <si>
+    <t>refrigerant</t>
+  </si>
+  <si>
+    <t>Refrigerant</t>
+  </si>
+  <si>
+    <t>Refrigerante</t>
+  </si>
+  <si>
+    <t>high_low_pressure_switch</t>
+  </si>
+  <si>
+    <t>High/Low Pressure Switch</t>
+  </si>
+  <si>
+    <t>interruptor de alta/baja presión</t>
   </si>
 </sst>
 </file>
@@ -992,7 +983,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1035,6 +1026,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="41">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1536,8 +1528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1577,7 +1569,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -1586,7 +1578,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -1724,20 +1716,20 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="1" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="J8" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -1786,10 +1778,10 @@
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="J11" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
@@ -1841,7 +1833,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C14" s="1"/>
       <c r="J14" s="9"/>
@@ -1849,22 +1841,22 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C15" s="1" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E15" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="F15" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="G15" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="I15" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="K15" s="9"/>
     </row>
@@ -1881,7 +1873,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C17" s="1"/>
       <c r="J17" s="9"/>
@@ -1916,7 +1908,7 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C19" s="1"/>
       <c r="J19" s="9"/>
@@ -1924,22 +1916,22 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C20" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="E20" t="s">
+        <v>202</v>
+      </c>
+      <c r="F20" t="s">
+        <v>203</v>
+      </c>
+      <c r="G20" t="s">
         <v>204</v>
       </c>
-      <c r="E20" t="s">
-        <v>211</v>
-      </c>
-      <c r="F20" t="s">
-        <v>212</v>
-      </c>
-      <c r="G20" t="s">
-        <v>213</v>
-      </c>
       <c r="I20" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="K20" s="9"/>
     </row>
@@ -1953,22 +1945,22 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C22" s="1" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E22" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="F22" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="G22" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="I22" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="K22" s="9"/>
     </row>
@@ -1985,7 +1977,7 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="C24" s="1"/>
       <c r="J24" s="9"/>
@@ -2008,31 +2000,31 @@
         <v>121</v>
       </c>
       <c r="I25" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C26" s="1" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E26" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="F26" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="G26" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="I26" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="K26" s="9"/>
     </row>
@@ -2077,10 +2069,10 @@
         <v>90</v>
       </c>
       <c r="I30" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="K30" s="9"/>
     </row>
@@ -2089,7 +2081,7 @@
         <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F31" t="s">
         <v>79</v>
@@ -2098,10 +2090,10 @@
         <v>85</v>
       </c>
       <c r="I31" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="J31" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -2111,19 +2103,19 @@
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C33" t="s">
+        <v>218</v>
+      </c>
+      <c r="F33" t="s">
+        <v>225</v>
+      </c>
+      <c r="G33" t="s">
+        <v>219</v>
+      </c>
+      <c r="I33" t="s">
+        <v>226</v>
+      </c>
+      <c r="J33" t="s">
         <v>227</v>
-      </c>
-      <c r="F33" t="s">
-        <v>234</v>
-      </c>
-      <c r="G33" t="s">
-        <v>228</v>
-      </c>
-      <c r="I33" t="s">
-        <v>235</v>
-      </c>
-      <c r="J33" t="s">
-        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -2139,10 +2131,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2168,7 +2160,7 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -2260,13 +2252,13 @@
         <v>91</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C10" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
@@ -2274,13 +2266,13 @@
         <v>91</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C11" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -2288,13 +2280,13 @@
         <v>91</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C12" t="s">
         <v>142</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -2302,13 +2294,13 @@
         <v>91</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C13" t="s">
         <v>143</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
@@ -2316,13 +2308,13 @@
         <v>91</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
@@ -2330,41 +2322,41 @@
         <v>91</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C15" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="C16" t="s">
-        <v>144</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="B16" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="C17" t="s">
-        <v>145</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>170</v>
+      <c r="B17" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
@@ -2372,13 +2364,13 @@
         <v>91</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="C18" t="s">
-        <v>159</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>171</v>
+        <v>144</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
@@ -2386,41 +2378,42 @@
         <v>91</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C19" t="s">
-        <v>146</v>
+        <v>165</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="C20" t="s">
-        <v>174</v>
-      </c>
-      <c r="D20" s="16" t="s">
-        <v>173</v>
-      </c>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="C21" t="s">
+        <v>178</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="E21" s="17"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>96</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C22" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="E22" s="17"/>
     </row>
@@ -2429,13 +2422,13 @@
         <v>96</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="C23" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E23" s="17"/>
     </row>
@@ -2444,13 +2437,13 @@
         <v>96</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="C24" t="s">
-        <v>193</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>194</v>
+        <v>187</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>188</v>
       </c>
       <c r="E24" s="17"/>
     </row>
@@ -2459,13 +2452,13 @@
         <v>96</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C25" t="s">
-        <v>196</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>197</v>
+        <v>190</v>
+      </c>
+      <c r="D25" t="s">
+        <v>190</v>
       </c>
       <c r="E25" s="17"/>
     </row>
@@ -2474,13 +2467,13 @@
         <v>96</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C26" t="s">
-        <v>199</v>
-      </c>
-      <c r="D26" t="s">
-        <v>199</v>
+        <v>192</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>193</v>
       </c>
       <c r="E26" s="17"/>
     </row>
@@ -2489,75 +2482,74 @@
         <v>96</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>200</v>
+        <v>82</v>
       </c>
       <c r="C27" t="s">
-        <v>201</v>
+        <v>79</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>202</v>
+        <v>85</v>
       </c>
       <c r="E27" s="17"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C28" t="s">
-        <v>79</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="E28" s="17"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B29" s="15"/>
-      <c r="D29" s="9"/>
-    </row>
-    <row r="30" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="15"/>
+      <c r="D28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>243</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="18" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
         <v>99</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="D30" s="18" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="18" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="18" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
         <v>99</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="18" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
         <v>99</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.35">
@@ -2565,55 +2557,41 @@
         <v>99</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="18" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A34" s="18" t="s">
         <v>99</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="18" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
         <v>99</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" s="19" t="s">
-        <v>251</v>
-      </c>
-      <c r="C36" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="D36" s="21" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -2745,7 +2723,7 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="F1" t="s">
         <v>39</v>
@@ -2754,7 +2732,7 @@
         <v>40</v>
       </c>
       <c r="H1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -2811,7 +2789,7 @@
         <v>48</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -2825,21 +2803,21 @@
         <v>51</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="G9" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added total hours of operation questions for unit 1 and unit 2
</commit_message>
<xml_diff>
--- a/app/config/tables/cold_room_maintenance_logs/forms/cold_room_maintenance_logs/cold_room_maintenance_logs.xlsx
+++ b/app/config/tables/cold_room_maintenance_logs/forms/cold_room_maintenance_logs/cold_room_maintenance_logs.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="274">
   <si>
     <t>clause</t>
   </si>
@@ -821,6 +821,39 @@
   </si>
   <si>
     <t>interruptor de alta/baja presión</t>
+  </si>
+  <si>
+    <t>integer</t>
+  </si>
+  <si>
+    <t>total_hrs_of_operation_unit1</t>
+  </si>
+  <si>
+    <t>total_hrs_of_operation_unit2</t>
+  </si>
+  <si>
+    <t>Total Hours of Operation Unit 1</t>
+  </si>
+  <si>
+    <t>Total Hours of Operation Unit 2</t>
+  </si>
+  <si>
+    <t>Total de horas de operación unidad 1</t>
+  </si>
+  <si>
+    <t>Total de horas de operación unidad 2</t>
+  </si>
+  <si>
+    <t>Enter total hours of operation for unit 2</t>
+  </si>
+  <si>
+    <t>Enter total hours of operation for unit 1</t>
+  </si>
+  <si>
+    <t>Ingrese el total de horas de operación para la unidad 1</t>
+  </si>
+  <si>
+    <t>Ingrese el total de horas de operación para la unidad 2</t>
   </si>
 </sst>
 </file>
@@ -1526,10 +1559,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="I22" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2101,20 +2134,70 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.35">
-      <c r="C33" t="s">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="I34" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="J34" s="18" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="J35" s="18" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C37" t="s">
         <v>218</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F37" t="s">
         <v>225</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G37" t="s">
         <v>219</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I37" t="s">
         <v>226</v>
       </c>
-      <c r="J33" t="s">
+      <c r="J37" t="s">
         <v>227</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update cold room and refrigerator maintenance logs note fields and actions_taken
</commit_message>
<xml_diff>
--- a/app/config/tables/cold_room_maintenance_logs/forms/cold_room_maintenance_logs/cold_room_maintenance_logs.xlsx
+++ b/app/config/tables/cold_room_maintenance_logs/forms/cold_room_maintenance_logs/cold_room_maintenance_logs.xlsx
@@ -85,21 +85,6 @@
     <t>Fecha de Servicio</t>
   </si>
   <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Notas</t>
-  </si>
-  <si>
-    <t>Enter any extra notes</t>
-  </si>
-  <si>
-    <t>Notas extras</t>
-  </si>
-  <si>
     <t>end screen</t>
   </si>
   <si>
@@ -622,63 +607,15 @@
     <t>text</t>
   </si>
   <si>
-    <t>other_maintenance</t>
-  </si>
-  <si>
-    <t>Other Maintenance</t>
-  </si>
-  <si>
-    <t>Otro mantenimiento</t>
-  </si>
-  <si>
-    <t>Enter other maintenance</t>
-  </si>
-  <si>
-    <t>Ingrese otro mantenimiento</t>
-  </si>
-  <si>
     <t>selected(data('type_of_repair'), 'other')</t>
   </si>
   <si>
-    <t>other_repair</t>
-  </si>
-  <si>
-    <t>Other Repair</t>
-  </si>
-  <si>
-    <t>Otra Reparación</t>
-  </si>
-  <si>
-    <t>Enter other repair</t>
-  </si>
-  <si>
-    <t>Ingrese otra reparación</t>
-  </si>
-  <si>
-    <t>repair_activities</t>
-  </si>
-  <si>
-    <t>Repair Activities</t>
-  </si>
-  <si>
-    <t>Actividades de Reparacion</t>
-  </si>
-  <si>
     <t>Enter actions taken</t>
   </si>
   <si>
     <t>Ingrese las acciones tomadas</t>
   </si>
   <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Enter comments</t>
-  </si>
-  <si>
-    <t>Ingrese comentarios</t>
-  </si>
-  <si>
     <t>other_spare_parts</t>
   </si>
   <si>
@@ -718,12 +655,6 @@
     <t>Actualice el estado del cuarto frio según sea necesario</t>
   </si>
   <si>
-    <t>Comentarios</t>
-  </si>
-  <si>
-    <t>preventative_comments</t>
-  </si>
-  <si>
     <t>Select spare parts replaced/used</t>
   </si>
   <si>
@@ -854,6 +785,75 @@
   </si>
   <si>
     <t>Ingrese el total de horas de operación para la unidad 2</t>
+  </si>
+  <si>
+    <t>actions_taken</t>
+  </si>
+  <si>
+    <t>Actions Taken</t>
+  </si>
+  <si>
+    <t>Acciones tomadas</t>
+  </si>
+  <si>
+    <t>other_maintenance_notes</t>
+  </si>
+  <si>
+    <t>Additional Notes for Other Maintenance</t>
+  </si>
+  <si>
+    <t>Notas adicionales para otro mantenimiento</t>
+  </si>
+  <si>
+    <t>Enter additional notes for other maintenance</t>
+  </si>
+  <si>
+    <t>Ingrese notas adicionales para otro mantenimiento</t>
+  </si>
+  <si>
+    <t>other_repair_notes</t>
+  </si>
+  <si>
+    <t>Notes for Other Repair Maintenance</t>
+  </si>
+  <si>
+    <t>Notas para otro mantenimiento de reparación</t>
+  </si>
+  <si>
+    <t>Enter notes for other repair maintenance</t>
+  </si>
+  <si>
+    <t>Ingrese notas para otro mantenimiento de reparación</t>
+  </si>
+  <si>
+    <t>repair_notes</t>
+  </si>
+  <si>
+    <t>Additional Repair Notes</t>
+  </si>
+  <si>
+    <t>Notas de reparación adicionales</t>
+  </si>
+  <si>
+    <t>Enter additional repair notes</t>
+  </si>
+  <si>
+    <t>Ingrese notas de reparación adicionales</t>
+  </si>
+  <si>
+    <t>preventative_notes</t>
+  </si>
+  <si>
+    <t>Additional Preventative Maintenance Notes</t>
+  </si>
+  <si>
+    <t>Notas de mantenimiento preventivo adicionales</t>
+  </si>
+  <si>
+    <t>Enter additional preventative maintenance notes</t>
+  </si>
+  <si>
+    <t>Ingrese notas de mantenimiento preventivo adicionales</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1016,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1060,6 +1060,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="41">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -1528,27 +1531,27 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:4" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1561,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I22" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1571,10 +1574,10 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
     <col min="4" max="4" width="22.58203125" customWidth="1"/>
-    <col min="5" max="5" width="20.58203125" customWidth="1"/>
+    <col min="5" max="5" width="25.1640625" customWidth="1"/>
     <col min="6" max="6" width="32.83203125" customWidth="1"/>
     <col min="7" max="8" width="32.33203125" customWidth="1"/>
-    <col min="9" max="9" width="24.58203125" customWidth="1"/>
+    <col min="9" max="9" width="32.58203125" customWidth="1"/>
     <col min="10" max="11" width="39.5" customWidth="1"/>
     <col min="12" max="1027" width="8.5" customWidth="1"/>
   </cols>
@@ -1602,7 +1605,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -1611,7 +1614,7 @@
         <v>8</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -1657,19 +1660,19 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="G4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="I4" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="J4" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -1693,26 +1696,26 @@
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K6" s="14"/>
     </row>
@@ -1724,20 +1727,20 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="K7" s="1"/>
     </row>
@@ -1749,25 +1752,25 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="J8" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1797,7 +1800,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C11" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3" t="s">
@@ -1811,53 +1814,54 @@
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="J11" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" t="s">
-        <v>20</v>
-      </c>
-      <c r="J12" t="s">
-        <v>21</v>
-      </c>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="G12" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="I12" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="C13" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="F13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="G13" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I13" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="K13" s="9"/>
     </row>
@@ -1866,32 +1870,32 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C14" s="1"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="C15" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E15" t="s">
-        <v>196</v>
-      </c>
-      <c r="F15" t="s">
-        <v>197</v>
-      </c>
-      <c r="G15" t="s">
-        <v>198</v>
-      </c>
-      <c r="I15" t="s">
-        <v>199</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="K15" s="9"/>
+    <row r="15" spans="1:12" s="18" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="C15" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>256</v>
+      </c>
+      <c r="I15" s="18" t="s">
+        <v>257</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="K15" s="21"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -1906,7 +1910,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="C17" s="1"/>
       <c r="J17" s="9"/>
@@ -1914,25 +1918,25 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C18" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D18" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E18" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G18" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="I18" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="K18" s="9"/>
     </row>
@@ -1941,32 +1945,32 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C19" s="1"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C20" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E20" t="s">
-        <v>202</v>
-      </c>
-      <c r="F20" t="s">
-        <v>203</v>
-      </c>
-      <c r="G20" t="s">
-        <v>204</v>
-      </c>
-      <c r="I20" t="s">
-        <v>205</v>
-      </c>
-      <c r="J20" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="K20" s="9"/>
+    <row r="20" spans="1:11" s="18" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="C20" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>262</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="K20" s="21"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
@@ -1976,26 +1980,25 @@
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C22" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E22" t="s">
-        <v>207</v>
-      </c>
-      <c r="F22" t="s">
-        <v>208</v>
-      </c>
-      <c r="G22" t="s">
-        <v>209</v>
-      </c>
-      <c r="I22" t="s">
-        <v>210</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="K22" s="9"/>
+    <row r="22" spans="1:11" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>264</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>265</v>
+      </c>
+      <c r="G22" s="18" t="s">
+        <v>266</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -2010,7 +2013,7 @@
         <v>11</v>
       </c>
       <c r="B24" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
       <c r="C24" s="1"/>
       <c r="J24" s="9"/>
@@ -2018,48 +2021,48 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C25" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" t="s">
+        <v>94</v>
+      </c>
+      <c r="E25" t="s">
         <v>95</v>
       </c>
-      <c r="D25" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" t="s">
-        <v>100</v>
-      </c>
       <c r="F25" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="G25" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="I25" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="K25" s="9"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C26" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="E26" t="s">
-        <v>229</v>
-      </c>
-      <c r="F26" t="s">
-        <v>212</v>
-      </c>
-      <c r="G26" t="s">
-        <v>228</v>
-      </c>
-      <c r="I26" t="s">
-        <v>213</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="K26" s="9"/>
+    <row r="26" spans="1:11" s="18" customFormat="1" ht="31" x14ac:dyDescent="0.35">
+      <c r="C26" s="23" t="s">
+        <v>190</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="J26" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="K26" s="21"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
@@ -2071,7 +2074,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C28" s="1"/>
       <c r="J28" s="9"/>
@@ -2087,25 +2090,25 @@
     </row>
     <row r="30" spans="1:11" ht="31" x14ac:dyDescent="0.35">
       <c r="C30" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E30" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F30" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G30" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I30" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="K30" s="9"/>
     </row>
@@ -2114,24 +2117,24 @@
         <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="F31" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G31" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="I31" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="J31" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
@@ -2141,64 +2144,64 @@
     </row>
     <row r="34" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C34" s="18" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>264</v>
+        <v>241</v>
       </c>
       <c r="F34" s="18" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="I34" s="18" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C35" s="18" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
       <c r="F35" s="18" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="G35" s="18" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="I35" s="18" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="J35" s="18" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C37" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="F37" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="G37" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="I37" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="J37" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -2231,10 +2234,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
@@ -2243,335 +2246,335 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
         <v>76</v>
       </c>
-      <c r="B3" t="s">
-        <v>81</v>
-      </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D6" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" t="s">
         <v>113</v>
-      </c>
-      <c r="D7" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" t="s">
         <v>114</v>
-      </c>
-      <c r="C8" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C10" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C11" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>157</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>260</v>
+        <v>237</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>261</v>
+        <v>238</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>262</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>257</v>
+        <v>234</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>258</v>
+        <v>235</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>259</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C18" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C19" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C21" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E21" s="17"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C22" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E22" s="17"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C23" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E23" s="17"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C24" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E24" s="17"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C25" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D25" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E25" s="17"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="C26" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E26" s="17"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C27" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E27" s="17"/>
     </row>
@@ -2581,100 +2584,100 @@
     </row>
     <row r="29" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="1:5" s="18" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="D30" s="21" t="s">
-        <v>251</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="18" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="D31" s="21" t="s">
-        <v>252</v>
+        <v>229</v>
       </c>
     </row>
     <row r="32" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>246</v>
+        <v>223</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>253</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>247</v>
+        <v>224</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>254</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="18" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A34" s="18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>248</v>
+        <v>225</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="C35" s="20" t="s">
-        <v>249</v>
+        <v>226</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>256</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -2711,54 +2714,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2794,10 +2797,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -2806,48 +2809,48 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="G1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B5" s="6">
         <v>20191005</v>
@@ -2855,7 +2858,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>14</v>
@@ -2863,44 +2866,44 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H7" s="17" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="G9" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -2933,138 +2936,138 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>55</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>